<commit_message>
updated certification script. added bmf gtd and stop market scenarios
</commit_message>
<xml_diff>
--- a/Fix/docs/certification_script.xlsx
+++ b/Fix/docs/certification_script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="814" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="814" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Swing Trade - Day" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="158">
   <si>
     <t>Item</t>
   </si>
@@ -487,6 +487,27 @@
   </si>
   <si>
     <t>l1</t>
+  </si>
+  <si>
+    <t>c11</t>
+  </si>
+  <si>
+    <t>Enviar um NewOrderSingle (OrdType = Stop) na compra de 100 a com o stop em R$2 e sem a tag price price,  com validade para o dia e TargetStrategy = 1002</t>
+  </si>
+  <si>
+    <t>Receber um ExecutionReport com ExecType = PendingNew, e logo após receber um outro ExecutionReport com o ExecType = New e OrdType = Stop. A tag Price devera informara o preco definido para o Stop.</t>
+  </si>
+  <si>
+    <t>g13</t>
+  </si>
+  <si>
+    <t>Enviar um NewOrderSingle (OrdType = Stop) na compra de 100 a com o stop em R$2 e sem a tag price price,  com validade para o dia</t>
+  </si>
+  <si>
+    <t>Enviar um NewOrderSingle na compra de um ativo da BMF, com validade para amanha</t>
+  </si>
+  <si>
+    <t>b7</t>
   </si>
 </sst>
 </file>
@@ -1161,7 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1209,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,6 +1338,19 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1325,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,6 +1518,19 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1977,10 +2024,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E14"/>
+  <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,6 +2210,19 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>